<commit_message>
support for special note and reference fields in excel added
</commit_message>
<xml_diff>
--- a/static/sample.xlsx
+++ b/static/sample.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/node-js/givezakat/static/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/givezakat/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FE196B-E42B-884A-A518-504915A97D9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FDE533C-9521-5F47-81AC-8069BCBABD67}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="31600" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="5660" windowWidth="28800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Earning per month</t>
   </si>
@@ -49,36 +49,6 @@
     <t>Currency</t>
   </si>
   <si>
-    <t>PKR</t>
-  </si>
-  <si>
-    <t>Pakistan</t>
-  </si>
-  <si>
-    <t>USA</t>
-  </si>
-  <si>
-    <t>USD</t>
-  </si>
-  <si>
-    <t>GBP</t>
-  </si>
-  <si>
-    <t>England</t>
-  </si>
-  <si>
-    <t>Austarlia</t>
-  </si>
-  <si>
-    <t>AUD</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>CAD</t>
-  </si>
-  <si>
     <t>Occupation</t>
   </si>
   <si>
@@ -86,6 +56,9 @@
   </si>
   <si>
     <t>Story</t>
+  </si>
+  <si>
+    <t>Remarks</t>
   </si>
 </sst>
 </file>
@@ -489,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,7 +482,7 @@
     <col min="10" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -523,22 +496,25 @@
         <v>0</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -547,7 +523,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -556,7 +532,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -565,7 +541,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -574,7 +550,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -583,7 +559,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -592,7 +568,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -601,7 +577,7 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -610,7 +586,7 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -619,7 +595,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -628,7 +604,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -637,7 +613,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -646,7 +622,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -655,7 +631,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -664,7 +640,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -962,7 +938,7 @@
           <x14:formula1>
             <xm:f>Sheet2!$B$1:$B$36</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E37</xm:sqref>
+          <xm:sqref>E31:E37</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -972,55 +948,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A6" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>